<commit_message>
d3 integration & test plot
</commit_message>
<xml_diff>
--- a/data/TestDataReduced.xlsx
+++ b/data/TestDataReduced.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phillip\Prototype\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dragan\Desktop\Coding\Prototype\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB747E4D-5ED1-4CBB-BDFD-84B1147695E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11954041-B4AB-4792-AD84-601ED4D8CF9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="888" windowWidth="24216" windowHeight="14400" xr2:uid="{2EAF2FF9-AFE1-45CB-BA33-B71752CE3960}"/>
+    <workbookView xWindow="2955" yWindow="0" windowWidth="21600" windowHeight="11235" xr2:uid="{2EAF2FF9-AFE1-45CB-BA33-B71752CE3960}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>E:"Dreiecke und Vierecke II"</t>
-  </si>
-  <si>
-    <t>Potenzen I</t>
   </si>
   <si>
     <t>Note der Abschlussprüfung</t>
@@ -818,6 +815,15 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -830,6 +836,18 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -838,30 +856,9 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -877,7 +874,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1176,207 +1173,205 @@
   <dimension ref="A1:AO28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="Z1" sqref="Z1:AB1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="37" width="4.33203125" customWidth="1"/>
+    <col min="2" max="37" width="4.28515625" customWidth="1"/>
     <col min="38" max="38" width="11" customWidth="1"/>
-    <col min="39" max="41" width="4.33203125" customWidth="1"/>
+    <col min="39" max="41" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="38" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="42"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="38" t="s">
+      <c r="L1" s="42"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="39"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="38" t="s">
+      <c r="O1" s="42"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="39"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="38" t="s">
+      <c r="R1" s="42"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="39"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="38" t="s">
+      <c r="U1" s="42"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="42"/>
+      <c r="AB1" s="43"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="43"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="42"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="42"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="40"/>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="45"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="40"/>
     </row>
-    <row r="2" spans="1:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="K2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="N2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="Q2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="T2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="W2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="Z2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="AC2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="AF2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AH2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="AI2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AK2" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="AL2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AM2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AN2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AN2" s="10" t="s">
+      <c r="AO2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="AO2" s="11" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="13">
         <v>3</v>
@@ -1457,7 +1452,7 @@
       <c r="AJ3" s="14"/>
       <c r="AK3" s="15"/>
       <c r="AL3" s="16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AM3" s="17">
         <f t="shared" ref="AM3:AO27" si="0">DP3</f>
@@ -1472,9 +1467,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="21">
         <v>1</v>
@@ -1486,7 +1481,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="22">
         <v>2</v>
@@ -1568,9 +1563,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="21">
         <v>3</v>
@@ -1609,7 +1604,7 @@
         <v>35</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O5" s="22">
         <v>2</v>
@@ -1651,7 +1646,7 @@
       <c r="AJ5" s="22"/>
       <c r="AK5" s="23"/>
       <c r="AL5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM5" s="25">
         <f t="shared" si="0"/>
@@ -1666,12 +1661,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="22">
         <v>3</v>
@@ -1716,13 +1711,13 @@
         <v>79</v>
       </c>
       <c r="Q6" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R6" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S6" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T6" s="21">
         <v>0</v>
@@ -1749,7 +1744,7 @@
       <c r="AJ6" s="22"/>
       <c r="AK6" s="23"/>
       <c r="AL6" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM6" s="25">
         <f t="shared" si="0"/>
@@ -1764,9 +1759,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="21">
         <v>1</v>
@@ -1787,13 +1782,13 @@
         <v>44</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="22">
         <v>1</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K7" s="21">
         <v>2</v>
@@ -1802,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O7" s="22">
         <v>1</v>
@@ -1814,22 +1809,22 @@
         <v>37</v>
       </c>
       <c r="Q7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R7" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S7" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U7" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V7" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W7" s="21"/>
       <c r="X7" s="22"/>
@@ -1860,9 +1855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="21">
         <v>3</v>
@@ -1874,7 +1869,7 @@
         <v>68</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" s="22">
         <v>3</v>
@@ -1892,16 +1887,16 @@
         <v>60</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O8" s="22">
         <v>1</v>
@@ -1943,7 +1938,7 @@
       <c r="AJ8" s="22"/>
       <c r="AK8" s="23"/>
       <c r="AL8" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM8" s="25">
         <f t="shared" si="0"/>
@@ -1958,9 +1953,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" s="21">
         <v>1</v>
@@ -2041,7 +2036,7 @@
       <c r="AJ9" s="22"/>
       <c r="AK9" s="23"/>
       <c r="AL9" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM9" s="25">
         <f t="shared" si="0"/>
@@ -2056,9 +2051,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="21">
         <v>3</v>
@@ -2067,10 +2062,10 @@
         <v>3</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="22">
         <v>3</v>
@@ -2088,10 +2083,10 @@
         <v>80</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M10" s="23">
         <v>90</v>
@@ -2115,10 +2110,10 @@
         <v>70</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U10" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V10" s="23">
         <v>100</v>
@@ -2139,7 +2134,7 @@
       <c r="AJ10" s="22"/>
       <c r="AK10" s="23"/>
       <c r="AL10" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AM10" s="25">
         <f t="shared" si="0"/>
@@ -2154,9 +2149,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="21">
         <v>3</v>
@@ -2237,7 +2232,7 @@
       <c r="AJ11" s="22"/>
       <c r="AK11" s="23"/>
       <c r="AL11" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM11" s="25">
         <f t="shared" si="0"/>
@@ -2252,9 +2247,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="21">
         <v>3</v>
@@ -2335,7 +2330,7 @@
       <c r="AJ12" s="22"/>
       <c r="AK12" s="23"/>
       <c r="AL12" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM12" s="25">
         <f t="shared" si="0"/>
@@ -2350,9 +2345,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="21">
         <v>3</v>
@@ -2433,7 +2428,7 @@
       <c r="AJ13" s="22"/>
       <c r="AK13" s="23"/>
       <c r="AL13" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM13" s="25">
         <f t="shared" si="0"/>
@@ -2448,9 +2443,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="21">
         <v>3</v>
@@ -2462,7 +2457,7 @@
         <v>61</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="22">
         <v>3</v>
@@ -2489,7 +2484,7 @@
         <v>90</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O14" s="22">
         <v>3</v>
@@ -2531,7 +2526,7 @@
       <c r="AJ14" s="22"/>
       <c r="AK14" s="23"/>
       <c r="AL14" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AM14" s="25">
         <f t="shared" si="0"/>
@@ -2546,9 +2541,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="21">
         <v>3</v>
@@ -2557,10 +2552,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="22">
         <v>3</v>
@@ -2578,10 +2573,10 @@
         <v>45</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M15" s="23">
         <v>25</v>
@@ -2605,10 +2600,10 @@
         <v>60</v>
       </c>
       <c r="T15" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U15" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V15" s="23">
         <v>43</v>
@@ -2629,7 +2624,7 @@
       <c r="AJ15" s="22"/>
       <c r="AK15" s="23"/>
       <c r="AL15" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AM15" s="25">
         <f t="shared" si="0"/>
@@ -2644,9 +2639,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="21">
         <v>3</v>
@@ -2727,7 +2722,7 @@
       <c r="AJ16" s="22"/>
       <c r="AK16" s="23"/>
       <c r="AL16" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM16" s="25">
         <f t="shared" si="0"/>
@@ -2742,9 +2737,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="21">
         <v>1</v>
@@ -2825,7 +2820,7 @@
       <c r="AJ17" s="22"/>
       <c r="AK17" s="23"/>
       <c r="AL17" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM17" s="25">
         <f t="shared" si="0"/>
@@ -2840,12 +2835,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="22">
         <v>3</v>
@@ -2890,16 +2885,16 @@
         <v>95</v>
       </c>
       <c r="Q18" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R18" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S18" s="23">
         <v>75</v>
       </c>
       <c r="T18" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="U18" s="22">
         <v>4</v>
@@ -2923,7 +2918,7 @@
       <c r="AJ18" s="22"/>
       <c r="AK18" s="23"/>
       <c r="AL18" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AM18" s="25">
         <f t="shared" si="0"/>
@@ -2938,9 +2933,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="21">
         <v>1</v>
@@ -3021,7 +3016,7 @@
       <c r="AJ19" s="22"/>
       <c r="AK19" s="23"/>
       <c r="AL19" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AM19" s="25">
         <f t="shared" si="0"/>
@@ -3036,9 +3031,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="21">
         <v>3</v>
@@ -3119,7 +3114,7 @@
       <c r="AJ20" s="22"/>
       <c r="AK20" s="28"/>
       <c r="AL20" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM20" s="25">
         <f t="shared" si="0"/>
@@ -3134,9 +3129,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="30">
         <v>3</v>
@@ -3217,7 +3212,7 @@
       <c r="AJ21" s="31"/>
       <c r="AK21" s="23"/>
       <c r="AL21" s="32" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM21" s="25">
         <f t="shared" si="0"/>
@@ -3232,9 +3227,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="21">
         <v>2</v>
@@ -3315,7 +3310,7 @@
       <c r="AJ22" s="22"/>
       <c r="AK22" s="23"/>
       <c r="AL22" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AM22" s="25">
         <f t="shared" si="0"/>
@@ -3330,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="20"/>
       <c r="B23" s="21"/>
       <c r="C23" s="22"/>
@@ -3382,9 +3377,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="22"/>
@@ -3436,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" s="20"/>
       <c r="B25" s="21"/>
       <c r="C25" s="22"/>
@@ -3488,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" s="20"/>
       <c r="B26" s="21"/>
       <c r="C26" s="22"/>
@@ -3540,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
@@ -3592,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:41" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:41" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="33"/>
       <c r="B28" s="34"/>
       <c r="C28" s="35"/>
@@ -3646,6 +3641,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
     <mergeCell ref="AM1:AO1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="W1:Y1"/>
@@ -3653,12 +3654,6 @@
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>